<commit_message>
Initilize motors and selinoids
Initilize every subsystems functions
</commit_message>
<xml_diff>
--- a/7432_2019_Hardware_ID.xlsx
+++ b/7432_2019_Hardware_ID.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcibam\Documents\GitHub\DeepSpace\FRC7432_DeepSpace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{91A58655-937C-4DEA-B1AB-D1A1DC8A3761}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39327429-12FF-4B2A-B595-ADCC6A79A772}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{E4B7A93B-49AA-4EB5-A461-7A3613D56331}"/>
   </bookViews>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA92944-2D88-4CE0-BB91-79309312C1F4}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>